<commit_message>
Update Excel files with improved styling: alternating row colors, cell padding, and auto-fit row heights
</commit_message>
<xml_diff>
--- a/solutions/aws/ai/intelligent-document-processing/delivery/communication-plan.xlsx
+++ b/solutions/aws/ai/intelligent-document-processing/delivery/communication-plan.xlsx
@@ -563,7 +563,7 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>November 09, 2025</t>
+          <t>November 13, 2025</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="26" customHeight="1">
+    <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
           <t>COMM-005</t>
@@ -1137,7 +1137,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="26" customHeight="1">
+    <row r="7">
       <c r="A7" s="7" t="inlineStr">
         <is>
           <t>COMM-006</t>
@@ -1219,7 +1219,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="26" customHeight="1">
+    <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
           <t>COMM-007</t>
@@ -1301,7 +1301,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="26" customHeight="1">
+    <row r="9">
       <c r="A9" s="7" t="inlineStr">
         <is>
           <t>COMM-008</t>
@@ -1383,7 +1383,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="26" customHeight="1">
+    <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
           <t>COMM-009</t>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="26" customHeight="1">
+    <row r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>COMM-010</t>
@@ -1547,7 +1547,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="26" customHeight="1">
+    <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
           <t>COMM-011</t>
@@ -1629,7 +1629,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="26" customHeight="1">
+    <row r="13">
       <c r="A13" s="7" t="inlineStr">
         <is>
           <t>COMM-012</t>
@@ -1711,7 +1711,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="26" customHeight="1">
+    <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
           <t>COMM-013</t>
@@ -1793,7 +1793,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="26" customHeight="1">
+    <row r="15">
       <c r="A15" s="7" t="inlineStr">
         <is>
           <t>COMM-014</t>
@@ -1875,7 +1875,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="26" customHeight="1">
+    <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
           <t>COMM-015</t>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="26" customHeight="1">
+    <row r="17">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>COMM-016</t>
@@ -2039,7 +2039,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="26" customHeight="1">
+    <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
           <t>COMM-017</t>
@@ -2121,7 +2121,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="26" customHeight="1">
+    <row r="19">
       <c r="A19" s="7" t="inlineStr">
         <is>
           <t>COMM-018</t>
@@ -2203,7 +2203,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="26" customHeight="1">
+    <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
           <t>COMM-019</t>
@@ -2285,7 +2285,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="26" customHeight="1">
+    <row r="21">
       <c r="A21" s="7" t="inlineStr">
         <is>
           <t>COMM-020</t>
@@ -2367,7 +2367,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="26" customHeight="1">
+    <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
           <t>COMM-021</t>
@@ -2449,7 +2449,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="26" customHeight="1">
+    <row r="23">
       <c r="A23" s="7" t="inlineStr">
         <is>
           <t>COMM-022</t>

</xml_diff>